<commit_message>
Addition of PDMS contaminant series to database
Silicon added as basic elemental component and polydimethylsiloxane oligomer contaminant series added to LOBDbase

git-svn-id: file:///home/git/hedgehog.fhcrc.org/bioconductor/branches/RELEASE_3_5/madman/Rpacks/LOBSTAHS@130715 bc3139a8-67e5-0310-9ffc-ced21a209358
</commit_message>
<xml_diff>
--- a/inst/doc/xlsx/LOBSTAHS_adductHierarchies.xlsx
+++ b/inst/doc/xlsx/LOBSTAHS_adductHierarchies.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27907"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jrcollins/Code/LOBSTAHS/inst/doc/xlsx/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\R\LOBSTAHS-DEV\inst\doc\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="580" yWindow="460" windowWidth="26780" windowHeight="17060" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17730" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="LOBSTAHS_adductHierarchies" sheetId="5" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
+      <x14:workbookPr defaultImageDpi="330"/>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="80">
   <si>
     <t>DGCC</t>
   </si>
@@ -262,12 +262,18 @@
   </si>
   <si>
     <t>Navigate to the worksheet "LOBSTAHS_adductHierarchies", then export as a .csv with the filename "LOBSTAHS_adductHierarchies.csv"; this file can be sourced by specifying the file path in the LOBSTAHS database generation function generateLOBdbase()</t>
+  </si>
+  <si>
+    <t>Added PDMS Series</t>
+  </si>
+  <si>
+    <t>PDMS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -417,6 +423,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -744,19 +753,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE22"/>
+  <dimension ref="A1:AF22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="AC19" sqref="AC19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.83203125" customWidth="1"/>
+    <col min="1" max="1" width="15.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
       <c r="C1" s="4" t="s">
         <v>47</v>
       </c>
@@ -789,7 +798,7 @@
       <c r="AD1" s="4"/>
       <c r="AE1" s="4"/>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -883,8 +892,11 @@
       <c r="AE2" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="AF2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -958,7 +970,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -972,7 +984,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>32</v>
       </c>
@@ -1016,7 +1028,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>33</v>
       </c>
@@ -1030,7 +1042,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>34</v>
       </c>
@@ -1080,7 +1092,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>35</v>
       </c>
@@ -1109,7 +1121,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>36</v>
       </c>
@@ -1135,7 +1147,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>37</v>
       </c>
@@ -1176,7 +1188,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>38</v>
       </c>
@@ -1223,7 +1235,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>39</v>
       </c>
@@ -1267,7 +1279,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>40</v>
       </c>
@@ -1317,7 +1329,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -1400,7 +1412,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -1474,7 +1486,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -1523,8 +1535,11 @@
       <c r="AC16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AF16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -1607,7 +1622,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -1660,7 +1675,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -1737,7 +1752,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>27</v>
       </c>
@@ -1778,7 +1793,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>28</v>
       </c>
@@ -1792,7 +1807,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>29</v>
       </c>
@@ -1838,24 +1853,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.5" customWidth="1"/>
     <col min="2" max="2" width="74.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>66</v>
       </c>
@@ -1863,42 +1878,42 @@
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>3</v>
       </c>
@@ -1909,7 +1924,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>42327</v>
       </c>
@@ -1920,7 +1935,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>42344</v>
       </c>
@@ -1931,7 +1946,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>42403</v>
       </c>
@@ -1942,7 +1957,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>42607</v>
       </c>
@@ -1953,7 +1968,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>42624</v>
       </c>
@@ -1964,7 +1979,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>42709</v>
       </c>
@@ -1975,7 +1990,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>42719</v>
       </c>
@@ -1986,7 +2001,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>42758</v>
       </c>
@@ -1997,7 +2012,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>42769</v>
       </c>
@@ -2006,6 +2021,17 @@
       </c>
       <c r="C22" s="3" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>42779</v>
+      </c>
+      <c r="B23" t="s">
+        <v>78</v>
+      </c>
+      <c r="C23" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>